<commit_message>
almost working version, still some cards do not load, still using image as unique id
</commit_message>
<xml_diff>
--- a/aggregated_order_details.xlsx
+++ b/aggregated_order_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,27 +448,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://tcgplayer.com/product/296?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/104400?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250294?irclickid=z2N1PG2hyxyKWHgV6XVKNVrtUkHXsK3lrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/118420?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250319?irclickid=2Rz2KM2hyxyKWHgV6XVKNVrtUkHXsKwZrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/129564?Printing=Foil&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,27 +478,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250324?irclickid=zlKXZ92hyxyKWHgV6XVKNVrtUkHXsK3ZrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/161851?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250326?irclickid=zUYyxB2hyxyKWHgV6XVKNVrtUkHXsK3FrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/192640?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250331?irclickid=2q%3AXzf2hyxyKWHgV6XVKNVrtUkHXsK1trRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/206648?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -508,37 +508,37 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250334?irclickid=zSWyM%3A2hyxyKWHgV6XVKNVrtUkHXsK3JrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/214901?Printing=Foil&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250336?irclickid=278y4i2hyxyKWHgV6XVKNVrtUkHXsK3RrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/221822?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250337?irclickid=2P4xuW2hyxyKWHgV6XVKNVrtUkHXsK1ZrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/234341?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250339?irclickid=22cSWT2hyxyKWHgV6XVKNVrtUkHXsKwJrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/235146?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250340?irclickid=2DvQQh2hyxyKWHgV6XVKNVrtUkHXsK1hrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/273302?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/250341?irclickid=SU9Wfe2h0xyKWHgV6XVKNVrtUkHXsoXNrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/275172?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/264204?irclickid=Q-Ryh%3A2h1xyKWHgV6XVKNVrtUkHXsNxhrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/276325?&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/264212?irclickid=VW0RmV2h1xyKWHgV6XVKNVrtUkHXsNxtrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/3737?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,10 +588,650 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.tcgplayer.com/product/264234?irclickid=TJHRqQ2h1xyKWHgV6XVKNVrtUkHXsIS1rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+          <t>https://tcgplayer.com/product/456826?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
         </is>
       </c>
       <c r="B16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/457273?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/457276?Printing=Foil&amp;Language=English&amp;Condition=Near+Mint|Lightly+Played</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/480529?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/498469?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/499536?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/505595?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/507170?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/518140?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/518164?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/518165?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/519234?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/523074?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/523131?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/525885?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/525997?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/526053?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint|Lightly+Played</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/526074?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint|Lightly+Played</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/528290?Printing=Foil&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/528291?Printing=Foil&amp;Language=English&amp;Condition=Near+Mint|Lightly+Played</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/539453?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/544934?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/549566?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/7044?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint|Lightly+Played</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/7549?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/91038?Printing=Normal&amp;Language=English&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/95368?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://tcgplayer.com/product/95389?&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/113697?irclickid=VnzXRD2hUxyKWHgV6XVKNVrtUkHXse2FrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/113764?irclickid=XQGU%3AQ2h0xyKWHgV6XVKNVrtUkHXsoV1rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Lightly+Played|Near+Mint</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/133776/pokemon-sm-burning-shadows-burning-shadows-elite-trainer-box?page=1&amp;Language=English&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/138521?irclickid=V2fTjf2h3xyKWHgV6XVKNVrtUkHXsPQVrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/149040?irclickid=Xn0SoVz74xyKTwPUY-1ZYXXLUkCxj62trRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/185985?irclickid=z17X4n2k6xyKWHgV6XVKNVrtUkHXspSJrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189243?irclickid=yrs1S22hyxyKWHgV6XVKNVrtUkHXsKV5rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189256?irclickid=WzASaY2hyxyKWHgV6XVKNVrtUkHXsc21rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189307?irclickid=WalX8V2h0xyKWHgV6XVKNVrtUkHXsoyprRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189321?irclickid=SGdXj62k6xyKWHgV6XVKNVrtUkHXsrwlrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189322?irclickid=X4DQMk2k6xyKWHgV6XVKNVrtUkHXsrzprRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/189325?irclickid=SUITXf2k6xyKWHgV6XVKNVrtUkHXsrzdrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/195089?irclickid=TSkVpj2h0xyKWHgV6XVKNVrtUkHXsoURrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/197872?irclickid=zKuRsL2k6xyKWHgV6XVKNVrtUkHXsu0NrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/201252?irclickid=Ww%3AV97z7-xyKTwPUY-1ZYXXLUkCxg2x1rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/218791/pokemon-champions-path-champions-path-elite-trainer-box?page=1&amp;Language=English&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/226710/magic-commander-legends-ramos-dragon-engine-foil-etched?Language=English&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/234052?irclickid=1sa1sv2h1xyKWHgV6XVKNVrtUkHXsIwZrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/256138/pokemon-swsh09-brilliant-stars-brilliant-stars-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/277335/pokemon-swsh11-lost-origin-lost-origin-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/42543?irclickid=0j00IP2h3xyKWHgV6XVKNVrtUkHXsN3drRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/476451/pokemon-sv01-scarlet-and-violet-base-set-scarlet-and-violet-booster-pack?Language=English&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/478041?irclickid=y4gyBj2hyxyKWHgV6XVKNVrtUkHXsKXprRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/493974/pokemon-sv02-paldea-evolved-paldea-evolved-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/493976/pokemon-sv02-paldea-evolved-paldea-evolved-booster-pack?page=1&amp;Language=English&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/501264/pokemon-sv03-obsidian-flames-obsidian-flames-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/503313/pokemon-sv-scarlet-and-violet-151-151-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/512822/pokemon-sv04-paradox-rift-paradox-rift-booster-pack?page=1&amp;Language=English&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/517034?irclickid=SGb1X72hyxyKWHgV6XVKNVrtUkHXscT1rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/523929?irclickid=WtXwaE2hxxyKWHgV6XVKNVrtUkHXsvx5rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/528040/pokemon-sv-paldean-fates-paldean-fates-elite-trainer-box?Condition=Unopened&amp;Language=all&amp;page=1&amp;ListingType=standard</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/535174?irclickid=SSszWO2hzxyKWHgV6XVKNVrtUkHXsJSBrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/550140?irclickid=TckUCaz7-xyKTwPUY-1ZYXXLUkCxg2z5rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Holofoil&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/83684?irclickid=RbHVg-2hwxyKWHgV6XVKNVrtUkHXsLxRrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/83690?irclickid=R5cwI-2hwxyKWHgV6XVKNVrtUkHXsLxhrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/84357?irclickid=Wm9Xp-2hwxyKWHgV6XVKNVrtUkHXsLx9rRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://www.tcgplayer.com/product/84827?irclickid=VkR2uY2hUxyKWHgV6XVKNVrtUkHXse2hrRa%3AX80&amp;sharedid=&amp;irpid=4944541&amp;irgwc=1&amp;utm_source=impact&amp;utm_medium=affiliate&amp;utm_campaign=Scrydex&amp;Printing=Normal&amp;ListingType=standard&amp;page=1&amp;Condition=Near+Mint</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>